<commit_message>
Added some examples in email sendind
</commit_message>
<xml_diff>
--- a/Python/MathuraCorreo/correos.xlsx
+++ b/Python/MathuraCorreo/correos.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO CIAC\Documents\GITRepos\MyFiles\Python\MathuraCorreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITRepos\MyFiles\Python\MathuraCorreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12096"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Correo</t>
   </si>
@@ -35,16 +35,19 @@
     <t>Verde</t>
   </si>
   <si>
-    <t>elvis_avfc@hotmail.com</t>
-  </si>
-  <si>
     <t>Azul</t>
+  </si>
+  <si>
+    <t>luisfervillaalta@gmail.com</t>
+  </si>
+  <si>
+    <t>jesssortigoza@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,10 +86,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -371,20 +373,20 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -392,23 +394,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>